<commit_message>
Fixes due to latest changes in db model
</commit_message>
<xml_diff>
--- a/MUSE Reports/Reports.xlsx
+++ b/MUSE Reports/Reports.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MuseAnalytics\muse-patternmining\MUSE Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MuseAnalytics\github\muse-pattern-mining\MUSE Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="localhost_muse_analytics_reporting_invalid_filmdauer" localSheetId="1" hidden="1">'Invalid Filmdauer'!$A$1:$D$2</definedName>
-    <definedName name="localhost_muse_analytics_reporting_invalid_timecodes" localSheetId="0" hidden="1">'Invalid Timecodes'!$A$1:$F$12</definedName>
+    <definedName name="localhost_muse_analytics_reporting_invalid_timecodes" localSheetId="0" hidden="1">'Invalid Timecodes'!$A$1:$F$9</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,17 +30,17 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\Administrator\Documents\Meine Datenquellen\localhost muse_analytics reporting_invalid_filmdauer.odc" keepAlive="1" name="localhost muse_analytics reporting_invalid_filmdauer" description="Reports" type="5" refreshedVersion="5" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=muse_analytics;Data Source=localhost;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=MUSEANALYTICS;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;muse_analytics&quot;.&quot;dbo&quot;.&quot;reporting_invalid_filmdauer&quot;" commandType="3"/>
+  <connection id="1" keepAlive="1" name="localhost muse_analytics reporting_invalid_filmdauer" description="Reports" type="5" refreshedVersion="5" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=muse_analytics;Data Source=localhost;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=MUSEANALYTICS;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;muse_nightly_analytics&quot;.&quot;dbo&quot;.&quot;reporting_invalid_filmdauer&quot;" commandType="3"/>
   </connection>
-  <connection id="2" odcFile="C:\Users\Administrator\Documents\Meine Datenquellen\localhost muse_analytics reporting_invalid_timecodes.odc" keepAlive="1" name="localhost muse_analytics reporting_invalid_timecodes" description="Reports" type="5" refreshedVersion="5" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=muse_analytics;Data Source=localhost;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=MUSEANALYTICS;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;muse_analytics&quot;.&quot;dbo&quot;.&quot;reporting_invalid_timecodes&quot;" commandType="3"/>
+  <connection id="2" keepAlive="1" name="localhost muse_analytics reporting_invalid_timecodes" description="Reports" type="5" refreshedVersion="5" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=muse_analytics;Data Source=localhost;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=MUSEANALYTICS;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;muse_nightly_analytics&quot;.&quot;dbo&quot;.&quot;reporting_invalid_timecodes&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>FilmID</t>
   </si>
@@ -82,30 +82,6 @@
   </si>
   <si>
     <t>https://muse.informatik.uni-stuttgart.de/#/filme/92/rollen/1/kostueme/2</t>
-  </si>
-  <si>
-    <t>0 Testfilm</t>
-  </si>
-  <si>
-    <t>test kostüm</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>https://muse.informatik.uni-stuttgart.de/#/filme/97/rollen/1/kostueme/1</t>
-  </si>
-  <si>
-    <t>charaTest</t>
-  </si>
-  <si>
-    <t>https://muse.informatik.uni-stuttgart.de/#/filme/97/rollen/1/kostueme/5</t>
-  </si>
-  <si>
-    <t>chara3</t>
-  </si>
-  <si>
-    <t>https://muse.informatik.uni-stuttgart.de/#/filme/97/rollen/1/kostueme/6</t>
   </si>
   <si>
     <t>Freizeitoutfit 1</t>
@@ -243,8 +219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_localhost_muse_analytics_reporting_invalid_timecodes" displayName="Tabelle_localhost_muse_analytics_reporting_invalid_timecodes" ref="A1:F12" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_localhost_muse_analytics_reporting_invalid_timecodes" displayName="Tabelle_localhost_muse_analytics_reporting_invalid_timecodes" ref="A1:F9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F9"/>
   <tableColumns count="6">
     <tableColumn id="1" uniqueName="1" name="Filmtitel" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="Kostuemkurztext" queryTableFieldId="2"/>
@@ -533,18 +509,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -572,79 +548,76 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>-128</v>
+        <v>-238</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>-59</v>
+        <v>-588</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>-3540</v>
+        <v>-47</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>-59</v>
+        <v>-128</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,19 +625,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>-238</v>
+        <v>-451</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -672,19 +645,19 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>-451</v>
+        <v>-456</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -692,19 +665,19 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>-456</v>
+        <v>-472</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,76 +685,19 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>-546</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>-472</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>-546</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11">
-        <v>-588</v>
-      </c>
-      <c r="F11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12">
-        <v>-47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>